<commit_message>
Started building our parse table in Parser.h using a map
</commit_message>
<xml_diff>
--- a/Compiler/doc/Parse Table.xlsx
+++ b/Compiler/doc/Parse Table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hilli\Documents\GitHub\Klein-Compiler\Compiler\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justice\Desktop\Klein-Compiler\Compiler\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parse Table" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Revised Grammar" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="Revised Grammar" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr sourceFile="C:\Users\hilli\Documents\GitHub\Klein-Compiler\Compiler\doc\Revised Grammar.txt" delimited="0">
       <textFields>
         <textField/>
@@ -682,7 +682,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -739,10 +739,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,7 +761,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Revised Grammar" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Revised Grammar" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1060,7 +1060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -1068,55 +1068,55 @@
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="34.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="50.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="50.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="2" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="1.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="2" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.7265625" style="4"/>
+    <col min="26" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1126,20 +1126,20 @@
       <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5" t="s">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="5"/>
+      <c r="W1" s="6"/>
       <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>189</v>
       </c>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>190</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>191</v>
       </c>
@@ -1321,7 +1321,7 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>192</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>193</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>194</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>195</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>196</v>
       </c>
@@ -1493,7 +1493,7 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>197</v>
       </c>
@@ -1526,7 +1526,7 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>198</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>199</v>
       </c>
@@ -1598,7 +1598,7 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>200</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>201</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>202</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>203</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>204</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>205</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>206</v>
       </c>
@@ -1801,7 +1801,7 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>207</v>
       </c>
@@ -1830,7 +1830,7 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>208</v>
       </c>
@@ -1859,7 +1859,7 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>209</v>
       </c>
@@ -1888,7 +1888,7 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>210</v>
       </c>
@@ -1933,34 +1933,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="73.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>159</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>107</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>103</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>87</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>85</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>69</v>
       </c>
@@ -2509,11 +2509,11 @@
       <c r="C29" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>59</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -2869,7 +2869,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D46"/>
+  <autoFilter ref="A1:D46" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>